<commit_message>
Addotional chanes to plots + draw io diagrams
</commit_message>
<xml_diff>
--- a/eval-book-peptide-results.xlsx
+++ b/eval-book-peptide-results.xlsx
@@ -493,32 +493,32 @@
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>0.8051 ± 0.0871</t>
+          <t>0.81 ± 0.09</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>0.6808 ± 0.1732</t>
+          <t>0.68 ± 0.17</t>
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>0.6910 ± 0.1140</t>
+          <t>0.69 ± 0.11</t>
         </is>
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>0.5596 ± 0.2571</t>
+          <t>0.56 ± 0.26</t>
         </is>
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>0.5962 ± 0.2079</t>
+          <t>0.60 ± 0.21</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
         <is>
-          <t>0.4707 ± 0.2231</t>
+          <t>0.47 ± 0.22</t>
         </is>
       </c>
     </row>
@@ -530,32 +530,32 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.7196 ± 0.0255</t>
+          <t>0.72 ± 0.03</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.5255 ± 0.0648</t>
+          <t>0.53 ± 0.06</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0.6287 ± 0.0340</t>
+          <t>0.63 ± 0.03</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0.3102 ± 0.0689</t>
+          <t>0.31 ± 0.07</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>0.4103 ± 0.0740</t>
+          <t>0.41 ± 0.07</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>0.2759 ± 0.0495</t>
+          <t>0.28 ± 0.05</t>
         </is>
       </c>
     </row>
@@ -567,32 +567,32 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.5243 ± 0.0285</t>
+          <t>0.52 ± 0.03</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.0000 ± 0.0000</t>
+          <t>0.00 ± 0.00</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.0000 ± 0.0000</t>
+          <t>0.00 ± 0.00</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0.0000 ± 0.0000</t>
+          <t>0.00 ± 0.00</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>0.0000 ± 0.0000</t>
+          <t>0.00 ± 0.00</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>0.0000 ± 0.0000</t>
+          <t>0.00 ± 0.00</t>
         </is>
       </c>
     </row>
@@ -604,32 +604,32 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.5727 ± 0.0409</t>
+          <t>0.57 ± 0.04</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.0075 ± 0.0224</t>
+          <t>0.01 ± 0.02</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.1000 ± 0.3000</t>
+          <t>0.10 ± 0.30</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>0.0006 ± 0.0017</t>
+          <t>0.00 ± 0.00</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>0.0011 ± 0.0033</t>
+          <t>0.00 ± 0.00</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>0.0061 ± 0.0183</t>
+          <t>0.01 ± 0.02</t>
         </is>
       </c>
     </row>
@@ -641,32 +641,32 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.7299 ± 0.0198</t>
+          <t>0.73 ± 0.02</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.5669 ± 0.0363</t>
+          <t>0.57 ± 0.04</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.6396 ± 0.0347</t>
+          <t>0.64 ± 0.03</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>0.3595 ± 0.0485</t>
+          <t>0.36 ± 0.05</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>0.4588 ± 0.0444</t>
+          <t>0.46 ± 0.04</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>0.3112 ± 0.0431</t>
+          <t>0.31 ± 0.04</t>
         </is>
       </c>
     </row>
@@ -720,32 +720,32 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0.8563 ± 0.0833</t>
+          <t>0.86 ± 0.08</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.7742 ± 0.1306</t>
+          <t>0.77 ± 0.13</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0.7024 ± 0.1280</t>
+          <t>0.70 ± 0.13</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>0.7255 ± 0.2028</t>
+          <t>0.73 ± 0.20</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>0.7046 ± 0.1613</t>
+          <t>0.70 ± 0.16</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>0.5707 ± 0.2100</t>
+          <t>0.57 ± 0.21</t>
         </is>
       </c>
     </row>
@@ -757,32 +757,32 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0.9280 ± 0.0197</t>
+          <t>0.93 ± 0.02</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.8739 ± 0.0231</t>
+          <t>0.87 ± 0.02</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0.8800 ± 0.0245</t>
+          <t>0.88 ± 0.02</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>0.8093 ± 0.0412</t>
+          <t>0.81 ± 0.04</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>0.8426 ± 0.0273</t>
+          <t>0.84 ± 0.03</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>0.7707 ± 0.0377</t>
+          <t>0.77 ± 0.04</t>
         </is>
       </c>
     </row>
@@ -794,32 +794,32 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0.5915 ± 0.1092</t>
+          <t>0.59 ± 0.11</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.0885 ± 0.2655</t>
+          <t>0.09 ± 0.27</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>0.0854 ± 0.2562</t>
+          <t>0.09 ± 0.26</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>0.0844 ± 0.2533</t>
+          <t>0.08 ± 0.25</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>0.0849 ± 0.2547</t>
+          <t>0.08 ± 0.25</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>0.0774 ± 0.2323</t>
+          <t>0.08 ± 0.23</t>
         </is>
       </c>
     </row>
@@ -831,32 +831,32 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.6203 ± 0.0600</t>
+          <t>0.62 ± 0.06</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.0952 ± 0.0679</t>
+          <t>0.10 ± 0.07</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>0.3601 ± 0.2971</t>
+          <t>0.36 ± 0.30</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>0.0138 ± 0.0119</t>
+          <t>0.01 ± 0.01</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>0.0265 ± 0.0227</t>
+          <t>0.03 ± 0.02</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>0.0207 ± 0.0522</t>
+          <t>0.02 ± 0.05</t>
         </is>
       </c>
     </row>
@@ -868,32 +868,32 @@
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t>0.9325 ± 0.0185</t>
+          <t>0.93 ± 0.02</t>
         </is>
       </c>
       <c r="D12" s="2" t="inlineStr">
         <is>
-          <t>0.8776 ± 0.0246</t>
+          <t>0.88 ± 0.02</t>
         </is>
       </c>
       <c r="E12" s="2" t="inlineStr">
         <is>
-          <t>0.8820 ± 0.0191</t>
+          <t>0.88 ± 0.02</t>
         </is>
       </c>
       <c r="F12" s="2" t="inlineStr">
         <is>
-          <t>0.8160 ± 0.0486</t>
+          <t>0.82 ± 0.05</t>
         </is>
       </c>
       <c r="G12" s="2" t="inlineStr">
         <is>
-          <t>0.8468 ± 0.0270</t>
+          <t>0.85 ± 0.03</t>
         </is>
       </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>0.7769 ± 0.0357</t>
+          <t>0.78 ± 0.04</t>
         </is>
       </c>
     </row>
@@ -947,32 +947,32 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>0.8197 ± 0.1215</t>
+          <t>0.82 ± 0.12</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>0.7045 ± 0.2543</t>
+          <t>0.70 ± 0.25</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>0.6825 ± 0.1699</t>
+          <t>0.68 ± 0.17</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>0.6760 ± 0.3168</t>
+          <t>0.68 ± 0.32</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>0.6357 ± 0.2866</t>
+          <t>0.64 ± 0.29</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>0.5261 ± 0.2811</t>
+          <t>0.53 ± 0.28</t>
         </is>
       </c>
     </row>
@@ -984,32 +984,32 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>0.9401 ± 0.0190</t>
+          <t>0.94 ± 0.02</t>
         </is>
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>0.8811 ± 0.0178</t>
+          <t>0.88 ± 0.02</t>
         </is>
       </c>
       <c r="E15" s="2" t="inlineStr">
         <is>
-          <t>0.8860 ± 0.0275 *</t>
+          <t>0.89 ± 0.03 *</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>0.8210 ± 0.0364</t>
+          <t>0.82 ± 0.04</t>
         </is>
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>0.8515 ± 0.0204</t>
+          <t>0.85 ± 0.02</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>0.7832 ± 0.0294 *</t>
+          <t>0.78 ± 0.03 *</t>
         </is>
       </c>
     </row>
@@ -1021,32 +1021,32 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>0.7870 ± 0.0222</t>
+          <t>0.79 ± 0.02</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>0.6273 ± 0.0390</t>
+          <t>0.63 ± 0.04</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>0.8546 ± 0.0352</t>
+          <t>0.85 ± 0.04</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>0.4105 ± 0.0565</t>
+          <t>0.41 ± 0.06</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>0.5515 ± 0.0462</t>
+          <t>0.55 ± 0.05</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>0.4808 ± 0.0327</t>
+          <t>0.48 ± 0.03</t>
         </is>
       </c>
     </row>
@@ -1058,32 +1058,32 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.8672 ± 0.0202</t>
+          <t>0.87 ± 0.02</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.7626 ± 0.0336</t>
+          <t>0.76 ± 0.03</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0.8596 ± 0.0233</t>
+          <t>0.86 ± 0.02</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>0.6138 ± 0.0555</t>
+          <t>0.61 ± 0.06</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>0.7149 ± 0.0401</t>
+          <t>0.71 ± 0.04</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>0.6234 ± 0.0442</t>
+          <t>0.62 ± 0.04</t>
         </is>
       </c>
     </row>
@@ -1095,32 +1095,32 @@
       </c>
       <c r="C18" s="2" t="inlineStr">
         <is>
-          <t>0.9412 ± 0.0190 *</t>
+          <t>0.94 ± 0.02 *</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0.8798 ± 0.0196</t>
+          <t>0.88 ± 0.02</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>0.8750 ± 0.0224</t>
+          <t>0.87 ± 0.02</t>
         </is>
       </c>
       <c r="F18" s="2" t="inlineStr">
         <is>
-          <t>0.8232 ± 0.0350</t>
+          <t>0.82 ± 0.03</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>0.8479 ± 0.0233</t>
+          <t>0.85 ± 0.02</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>0.7763 ± 0.0334</t>
+          <t>0.78 ± 0.03</t>
         </is>
       </c>
     </row>
@@ -1142,7 +1142,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>0.0013</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">

</xml_diff>